<commit_message>
Datos Duros desde FA
</commit_message>
<xml_diff>
--- a/Sprints diarios.xlsx
+++ b/Sprints diarios.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$D$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Llegada a Datos Duros (Agregar) desde IM</t>
+  </si>
+  <si>
+    <t>Importar avatar de producto</t>
   </si>
 </sst>
 </file>
@@ -391,11 +394,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44461</v>
       </c>
@@ -467,6 +470,9 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -484,8 +490,19 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44461</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D6">
+  <autoFilter ref="A1:D7">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>